<commit_message>
STEP 8 + STEP 9. Final.
</commit_message>
<xml_diff>
--- a/Airport_data_frequency.xlsx
+++ b/Airport_data_frequency.xlsx
@@ -536,7 +536,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>1090</t>
+          <t>216</t>
         </is>
       </c>
     </row>
@@ -566,7 +566,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>895</t>
+          <t>504</t>
         </is>
       </c>
     </row>
@@ -596,7 +596,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>895</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -626,7 +626,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>3194</t>
+          <t>504</t>
         </is>
       </c>
     </row>
@@ -656,7 +656,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2734</t>
+          <t>216</t>
         </is>
       </c>
     </row>
@@ -686,7 +686,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>1492</t>
+          <t>288</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2727</t>
+          <t>144</t>
         </is>
       </c>
     </row>
@@ -745,7 +745,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -801,7 +801,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -829,7 +829,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>2522</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15">
@@ -857,7 +857,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>4100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16">
@@ -885,7 +885,7 @@
         </is>
       </c>
       <c r="F16" t="n">
-        <v>2727</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17">
@@ -913,7 +913,7 @@
         </is>
       </c>
       <c r="F17" t="n">
-        <v>895</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18">
@@ -941,7 +941,7 @@
         </is>
       </c>
       <c r="F18" t="n">
-        <v>3109</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19">
@@ -1000,7 +1000,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>3520</t>
+          <t>144</t>
         </is>
       </c>
     </row>
@@ -1030,7 +1030,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>2267</t>
+          <t>216</t>
         </is>
       </c>
     </row>
@@ -1060,7 +1060,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>1235</t>
+          <t>216</t>
         </is>
       </c>
     </row>
@@ -1090,7 +1090,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>3194</t>
+          <t>504</t>
         </is>
       </c>
     </row>
@@ -1120,7 +1120,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>3922</t>
+          <t>144</t>
         </is>
       </c>
     </row>
@@ -1150,7 +1150,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1180,7 +1180,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1240,7 +1240,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>1335</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -1270,7 +1270,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>1492</t>
+          <t>288</t>
         </is>
       </c>
     </row>
@@ -1300,7 +1300,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>1127</t>
+          <t>72</t>
         </is>
       </c>
     </row>
@@ -1330,7 +1330,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>4100</t>
+          <t>216</t>
         </is>
       </c>
     </row>
@@ -1360,7 +1360,7 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>4100</t>
+          <t>72</t>
         </is>
       </c>
     </row>
@@ -1390,7 +1390,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>2267</t>
+          <t>216</t>
         </is>
       </c>
     </row>
@@ -1420,7 +1420,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>2952</t>
+          <t>144</t>
         </is>
       </c>
     </row>
@@ -1480,7 +1480,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>2952</t>
+          <t>144</t>
         </is>
       </c>
     </row>
@@ -1510,7 +1510,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>2108</t>
+          <t>144</t>
         </is>
       </c>
     </row>
@@ -1540,7 +1540,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>2734</t>
+          <t>216</t>
         </is>
       </c>
     </row>
@@ -1570,7 +1570,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>2870</t>
+          <t>72</t>
         </is>
       </c>
     </row>
@@ -1600,7 +1600,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>2522</t>
+          <t>144</t>
         </is>
       </c>
     </row>
@@ -1630,7 +1630,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>2522</t>
+          <t>72</t>
         </is>
       </c>
     </row>
@@ -1660,7 +1660,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>3520</t>
+          <t>144</t>
         </is>
       </c>
     </row>
@@ -1720,7 +1720,7 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>3109</t>
+          <t>216</t>
         </is>
       </c>
     </row>
@@ -1750,7 +1750,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>3109</t>
+          <t>72</t>
         </is>
       </c>
     </row>
@@ -1780,7 +1780,7 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>3922</t>
+          <t>144</t>
         </is>
       </c>
     </row>
@@ -1810,7 +1810,7 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>2870</t>
+          <t>72</t>
         </is>
       </c>
     </row>
@@ -1840,7 +1840,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>1127</t>
+          <t>72</t>
         </is>
       </c>
     </row>
@@ -1870,7 +1870,7 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>1082</t>
+          <t>216</t>
         </is>
       </c>
     </row>
@@ -1900,7 +1900,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>1090</t>
+          <t>216</t>
         </is>
       </c>
     </row>
@@ -1960,7 +1960,7 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>2727</t>
+          <t>144</t>
         </is>
       </c>
     </row>
@@ -1990,7 +1990,7 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>1082</t>
+          <t>216</t>
         </is>
       </c>
     </row>
@@ -2020,7 +2020,7 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>2727</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2050,7 +2050,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>2727</t>
+          <t>144</t>
         </is>
       </c>
     </row>
@@ -2080,7 +2080,7 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>1235</t>
+          <t>216</t>
         </is>
       </c>
     </row>
@@ -2110,7 +2110,7 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>2108</t>
+          <t>144</t>
         </is>
       </c>
     </row>
@@ -2140,7 +2140,7 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>1335</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2200,7 +2200,7 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2230,7 +2230,7 @@
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2260,7 +2260,7 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>2522</t>
+          <t>144</t>
         </is>
       </c>
     </row>
@@ -2290,7 +2290,7 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>4100</t>
+          <t>216</t>
         </is>
       </c>
     </row>
@@ -2320,7 +2320,7 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>2727</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -2350,7 +2350,7 @@
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>895</t>
+          <t>504</t>
         </is>
       </c>
     </row>
@@ -2380,7 +2380,7 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>3109</t>
+          <t>216</t>
         </is>
       </c>
     </row>

</xml_diff>